<commit_message>
correção de erros, implementação de data de criação
</commit_message>
<xml_diff>
--- a/miro_dados_desde_janeiro.xlsx
+++ b/miro_dados_desde_janeiro.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y33"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,6 +559,11 @@
           <t>Término dos relatórios</t>
         </is>
       </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Data de criação</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -638,8 +643,21 @@
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>05/06/2024</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -719,8 +737,21 @@
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>18/06/2024</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -806,8 +837,21 @@
       <c r="W4" t="n">
         <v>839</v>
       </c>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>16/09/2024</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -893,8 +937,21 @@
       <c r="W5" t="n">
         <v>189</v>
       </c>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>01/10/2024</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -966,8 +1023,21 @@
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>16/10/2024</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1053,8 +1123,21 @@
       <c r="W7" t="n">
         <v>353</v>
       </c>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>16/09/2024</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1140,8 +1223,17 @@
       <c r="W8" t="n">
         <v>7760</v>
       </c>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1227,8 +1319,21 @@
       <c r="W9" t="n">
         <v>56</v>
       </c>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>16/09/2024</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1304,8 +1409,21 @@
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>05/06/2024</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1391,8 +1509,21 @@
       <c r="W11" t="n">
         <v>240</v>
       </c>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>16/09/2024</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1474,8 +1605,17 @@
       <c r="W12" t="n">
         <v>1499</v>
       </c>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1551,8 +1691,21 @@
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
       <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>05/06/2024</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1632,8 +1785,21 @@
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
       <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1713,8 +1879,17 @@
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
       <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1796,8 +1971,21 @@
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1877,8 +2065,17 @@
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1960,8 +2157,21 @@
       <c r="W18" t="n">
         <v>45</v>
       </c>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr"/>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>16/09/2024</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2041,8 +2251,21 @@
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
       <c r="W19" t="inlineStr"/>
-      <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="inlineStr"/>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2112,8 +2335,21 @@
       <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
       <c r="W20" t="inlineStr"/>
-      <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="inlineStr"/>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>15/10/2024</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2193,8 +2429,17 @@
       <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="inlineStr"/>
-      <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="inlineStr"/>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2274,8 +2519,21 @@
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
       <c r="W22" t="inlineStr"/>
-      <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="inlineStr"/>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z22" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2355,8 +2613,21 @@
       <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
-      <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="inlineStr"/>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2426,8 +2697,17 @@
       <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
-      <c r="X24" t="inlineStr"/>
-      <c r="Y24" t="inlineStr"/>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2507,8 +2787,17 @@
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
       <c r="W25" t="inlineStr"/>
-      <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="inlineStr"/>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2578,8 +2867,17 @@
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr"/>
       <c r="W26" t="inlineStr"/>
-      <c r="X26" t="inlineStr"/>
-      <c r="Y26" t="inlineStr"/>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2649,8 +2947,21 @@
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
       <c r="W27" t="inlineStr"/>
-      <c r="X27" t="inlineStr"/>
-      <c r="Y27" t="inlineStr"/>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z27" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2720,8 +3031,21 @@
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="inlineStr"/>
       <c r="W28" t="inlineStr"/>
-      <c r="X28" t="inlineStr"/>
-      <c r="Y28" t="inlineStr"/>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z28" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2791,8 +3115,17 @@
       <c r="U29" t="inlineStr"/>
       <c r="V29" t="inlineStr"/>
       <c r="W29" t="inlineStr"/>
-      <c r="X29" t="inlineStr"/>
-      <c r="Y29" t="inlineStr"/>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2858,8 +3191,21 @@
       <c r="U30" t="inlineStr"/>
       <c r="V30" t="inlineStr"/>
       <c r="W30" t="inlineStr"/>
-      <c r="X30" t="inlineStr"/>
-      <c r="Y30" t="inlineStr"/>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z30" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2939,8 +3285,21 @@
       <c r="U31" t="inlineStr"/>
       <c r="V31" t="inlineStr"/>
       <c r="W31" t="inlineStr"/>
-      <c r="X31" t="inlineStr"/>
-      <c r="Y31" t="inlineStr"/>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z31" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3010,8 +3369,21 @@
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="inlineStr"/>
       <c r="W32" t="inlineStr"/>
-      <c r="X32" t="inlineStr"/>
-      <c r="Y32" t="inlineStr"/>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z32" t="inlineStr">
+        <is>
+          <t>24/05/2024</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3075,8 +3447,17 @@
       <c r="U33" t="inlineStr"/>
       <c r="V33" t="inlineStr"/>
       <c r="W33" t="inlineStr"/>
-      <c r="X33" t="inlineStr"/>
-      <c r="Y33" t="inlineStr"/>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>30/10/2024</t>
+        </is>
+      </c>
+      <c r="Z33" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>